<commit_message>
Prueba con archivo modificado en carpeta.
</commit_message>
<xml_diff>
--- a/Excel_files/Data Base Fields.xlsx
+++ b/Excel_files/Data Base Fields.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t xml:space="preserve">LAB TESTS</t>
   </si>
@@ -80,6 +80,9 @@
   </si>
   <si>
     <t xml:space="preserve">INSTITUTE / HOSPITAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VEAMOS QUE PASA SI HAGO ESTO</t>
   </si>
 </sst>
 </file>
@@ -184,13 +187,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:R3"/>
+  <dimension ref="A2:R10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R3" activeCellId="0" sqref="R3"/>
+      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.75"/>
@@ -274,6 +277,11 @@
         <v>19</v>
       </c>
     </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="J2:K2"/>

</xml_diff>